<commit_message>
Start to adapt tier 1 to RD model. Adapt A1 and A2 scripts. Also, adapt yaml of those scripts. Add otoole into the Requierements file. Put de excel and pickle files with the RD data.
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Inputs/A-I_Horizon_Configuration.xlsx
+++ b/t1_confection/A1_Inputs/A-I_Horizon_Configuration.xlsx
@@ -403,4 +403,252 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
+    <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <xsd:import namespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="13" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B8FE9F-93E8-4D65-B59C-18304CD7A4D0}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB815CDD-081E-435E-8A65-3F13801F858B}"/>
 </file>
</xml_diff>

<commit_message>
Introduce the excel files of the JAM Energy model, also start to make a parametrization of the MOMF_T1_A.yaml
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Inputs/A-I_Horizon_Configuration.xlsx
+++ b/t1_confection/A1_Inputs/A-I_Horizon_Configuration.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\Dropbox\2_WORK\EperLab\5_Artículos EPERLab\0_In_progress\RESP\_multipurpose_model_fmwk\t1_confection\A1_Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisfernando\Dropbox\2_WORK\MOMF\JAM_Model_v1\1_3_Electricty_Buildings\A1_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A041FCF-D8C5-4885-BB5A-FA0A346AD78D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A27065-9A8B-455A-B950-32D15F11863B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-3855" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37260" yWindow="1140" windowWidth="18375" windowHeight="15255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Horizon" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -375,15 +386,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -391,12 +404,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="B2" s="2">
-        <v>2050</v>
+        <v>2055</v>
       </c>
     </row>
   </sheetData>
@@ -406,10 +419,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
-    <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-    <xsd:import namespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F74FB0E003A88C4B9D9793633BA4B356" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="0b91461ea42f649c0e2a912844849d59">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d55314f-45f1-40c9-9fce-63556e193d03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2dde1a2dc8a4a80923ccdd7c7b3969d3" ns2:_="">
+    <xsd:import namespace="0d55314f-45f1-40c9-9fce-63556e193d03"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -418,18 +430,15 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -437,7 +446,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0d55314f-45f1-40c9-9fce-63556e193d03" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -450,90 +459,53 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="13" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -546,8 +518,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -637,6 +609,16 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0d55314f-45f1-40c9-9fce-63556e193d03">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -646,9 +628,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B8FE9F-93E8-4D65-B59C-18304CD7A4D0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBAA7122-E54F-4E8A-B203-5C2FAB4C3517}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB815CDD-081E-435E-8A65-3F13801F858B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25A2AC8F-D36D-463A-B137-1935D135D22C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB815CDD-081E-435E-8A65-3F13801F858B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>